<commit_message>
update code for report.
</commit_message>
<xml_diff>
--- a/src/main/webapp/report/template_quotaion_client.xlsx
+++ b/src/main/webapp/report/template_quotaion_client.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luan/git/sanyo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luan/git/sanyo/src/main/webapp/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" tabRatio="806"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" tabRatio="806" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="cov" sheetId="8" r:id="rId1"/>
@@ -2615,7 +2615,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="355">
   <si>
     <t>a* :</t>
     <phoneticPr fontId="67"/>
@@ -5186,6 +5186,9 @@
       </rPr>
       <t xml:space="preserve">   (           months)</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">     </t>
   </si>
 </sst>
 </file>
@@ -7719,67 +7722,67 @@
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="246" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="247" applyFont="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="247" applyFont="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="84" fillId="0" borderId="22" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="84" fillId="0" borderId="14" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="23" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="24" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="25" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="1" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="7" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="34" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="35" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="36" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="42" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="43" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="44" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="77" fillId="0" borderId="33" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="23" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="24" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="25" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="84" fillId="0" borderId="23" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="247" applyFont="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="247" applyFont="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="84" fillId="0" borderId="22" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="84" fillId="0" borderId="14" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="1" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="7" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="34" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="35" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="36" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="42" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="43" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="44" xfId="247" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -7895,8 +7898,8 @@
     <cellStyle name="ÅëÈ­_ÿÿÿÿÿÿ" xfId="105"/>
     <cellStyle name="APPEAR" xfId="106"/>
     <cellStyle name="ÄÞ¸¶ [0]_±âÅ¸" xfId="107"/>
+    <cellStyle name="ÄÞ¸¶_±âÅ¸" xfId="109"/>
     <cellStyle name="AÞ¸¶ [0]_INQUIRY ¿?¾÷AßAø " xfId="108"/>
-    <cellStyle name="ÄÞ¸¶_±âÅ¸" xfId="109"/>
     <cellStyle name="AÞ¸¶_INQUIRY ¿?¾÷AßAø " xfId="110"/>
     <cellStyle name="Bad" xfId="111"/>
     <cellStyle name="C?AØ_¿?¾÷CoE² " xfId="112"/>
@@ -9674,7 +9677,7 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="C1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A9" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A24" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
@@ -10302,13 +10305,13 @@
       <c r="F2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="197" t="s">
+      <c r="G2" s="192" t="s">
         <v>152</v>
       </c>
-      <c r="H2" s="198"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="198"/>
-      <c r="K2" s="198"/>
+      <c r="H2" s="193"/>
+      <c r="I2" s="193"/>
+      <c r="J2" s="193"/>
+      <c r="K2" s="193"/>
     </row>
     <row r="3" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="20"/>
@@ -10371,13 +10374,13 @@
       <c r="A7" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="207" t="s">
+      <c r="B7" s="205" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="208"/>
-      <c r="D7" s="208"/>
-      <c r="E7" s="208"/>
-      <c r="F7" s="209"/>
+      <c r="C7" s="206"/>
+      <c r="D7" s="206"/>
+      <c r="E7" s="206"/>
+      <c r="F7" s="207"/>
       <c r="G7" s="169" t="s">
         <v>7</v>
       </c>
@@ -10398,13 +10401,13 @@
       <c r="A8" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="210" t="s">
+      <c r="B8" s="208" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="211"/>
-      <c r="D8" s="211"/>
-      <c r="E8" s="211"/>
-      <c r="F8" s="212"/>
+      <c r="C8" s="209"/>
+      <c r="D8" s="209"/>
+      <c r="E8" s="209"/>
+      <c r="F8" s="210"/>
       <c r="G8" s="170"/>
       <c r="H8" s="170"/>
       <c r="I8" s="170"/>
@@ -10529,7 +10532,7 @@
       <c r="H16" s="172"/>
       <c r="I16" s="172"/>
       <c r="J16" s="172"/>
-      <c r="K16" s="199"/>
+      <c r="K16" s="194"/>
     </row>
     <row r="17" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="36"/>
@@ -10544,7 +10547,7 @@
       <c r="H17" s="173"/>
       <c r="I17" s="170"/>
       <c r="J17" s="173"/>
-      <c r="K17" s="200"/>
+      <c r="K17" s="195"/>
     </row>
     <row r="18" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="31"/>
@@ -10803,13 +10806,13 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A35" s="31"/>
-      <c r="B35" s="193" t="s">
+      <c r="B35" s="196" t="s">
         <v>185</v>
       </c>
-      <c r="C35" s="194"/>
-      <c r="D35" s="194"/>
-      <c r="E35" s="194"/>
-      <c r="F35" s="195"/>
+      <c r="C35" s="197"/>
+      <c r="D35" s="197"/>
+      <c r="E35" s="197"/>
+      <c r="F35" s="198"/>
       <c r="G35" s="172"/>
       <c r="H35" s="172"/>
       <c r="I35" s="172"/>
@@ -10953,13 +10956,13 @@
     </row>
     <row r="45" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A45" s="71"/>
-      <c r="B45" s="193" t="s">
+      <c r="B45" s="196" t="s">
         <v>195</v>
       </c>
-      <c r="C45" s="194"/>
-      <c r="D45" s="194"/>
-      <c r="E45" s="194"/>
-      <c r="F45" s="194"/>
+      <c r="C45" s="197"/>
+      <c r="D45" s="197"/>
+      <c r="E45" s="197"/>
+      <c r="F45" s="197"/>
       <c r="G45" s="174"/>
       <c r="H45" s="172"/>
       <c r="I45" s="172"/>
@@ -11358,13 +11361,13 @@
     </row>
     <row r="72" spans="1:11" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="31"/>
-      <c r="B72" s="193" t="s">
+      <c r="B72" s="196" t="s">
         <v>219</v>
       </c>
-      <c r="C72" s="194"/>
-      <c r="D72" s="194"/>
-      <c r="E72" s="194"/>
-      <c r="F72" s="195"/>
+      <c r="C72" s="197"/>
+      <c r="D72" s="197"/>
+      <c r="E72" s="197"/>
+      <c r="F72" s="198"/>
       <c r="G72" s="176"/>
       <c r="H72" s="172"/>
       <c r="I72" s="181"/>
@@ -11373,13 +11376,13 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A73" s="45"/>
-      <c r="B73" s="204" t="s">
+      <c r="B73" s="202" t="s">
         <v>220</v>
       </c>
-      <c r="C73" s="205"/>
-      <c r="D73" s="205"/>
-      <c r="E73" s="205"/>
-      <c r="F73" s="206"/>
+      <c r="C73" s="203"/>
+      <c r="D73" s="203"/>
+      <c r="E73" s="203"/>
+      <c r="F73" s="204"/>
       <c r="G73" s="177"/>
       <c r="H73" s="173"/>
       <c r="I73" s="179"/>
@@ -11388,32 +11391,32 @@
     </row>
     <row r="74" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="77"/>
-      <c r="B74" s="201" t="s">
+      <c r="B74" s="199" t="s">
         <v>141</v>
       </c>
-      <c r="C74" s="202"/>
-      <c r="D74" s="202"/>
-      <c r="E74" s="202"/>
-      <c r="F74" s="202"/>
-      <c r="G74" s="202"/>
-      <c r="H74" s="202"/>
-      <c r="I74" s="202"/>
-      <c r="J74" s="203"/>
+      <c r="C74" s="200"/>
+      <c r="D74" s="200"/>
+      <c r="E74" s="200"/>
+      <c r="F74" s="200"/>
+      <c r="G74" s="200"/>
+      <c r="H74" s="200"/>
+      <c r="I74" s="200"/>
+      <c r="J74" s="201"/>
       <c r="K74" s="34"/>
     </row>
     <row r="75" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="77"/>
-      <c r="B75" s="201" t="s">
+      <c r="B75" s="199" t="s">
         <v>44</v>
       </c>
-      <c r="C75" s="202"/>
-      <c r="D75" s="202"/>
-      <c r="E75" s="202"/>
-      <c r="F75" s="202"/>
-      <c r="G75" s="202"/>
-      <c r="H75" s="202"/>
-      <c r="I75" s="202"/>
-      <c r="J75" s="203"/>
+      <c r="C75" s="200"/>
+      <c r="D75" s="200"/>
+      <c r="E75" s="200"/>
+      <c r="F75" s="200"/>
+      <c r="G75" s="200"/>
+      <c r="H75" s="200"/>
+      <c r="I75" s="200"/>
+      <c r="J75" s="201"/>
       <c r="K75" s="34"/>
     </row>
     <row r="76" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -11795,13 +11798,13 @@
     </row>
     <row r="101" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A101" s="31"/>
-      <c r="B101" s="193" t="s">
+      <c r="B101" s="196" t="s">
         <v>239</v>
       </c>
-      <c r="C101" s="194"/>
-      <c r="D101" s="194"/>
-      <c r="E101" s="194"/>
-      <c r="F101" s="195"/>
+      <c r="C101" s="197"/>
+      <c r="D101" s="197"/>
+      <c r="E101" s="197"/>
+      <c r="F101" s="198"/>
       <c r="G101" s="172"/>
       <c r="H101" s="172"/>
       <c r="I101" s="172"/>
@@ -12575,13 +12578,13 @@
     </row>
     <row r="153" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A153" s="31"/>
-      <c r="B153" s="193" t="s">
+      <c r="B153" s="196" t="s">
         <v>276</v>
       </c>
-      <c r="C153" s="194"/>
-      <c r="D153" s="194"/>
-      <c r="E153" s="194"/>
-      <c r="F153" s="195"/>
+      <c r="C153" s="197"/>
+      <c r="D153" s="197"/>
+      <c r="E153" s="197"/>
+      <c r="F153" s="198"/>
       <c r="G153" s="172"/>
       <c r="H153" s="172"/>
       <c r="I153" s="172"/>
@@ -13207,13 +13210,13 @@
     </row>
     <row r="193" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A193" s="31"/>
-      <c r="B193" s="193" t="s">
+      <c r="B193" s="196" t="s">
         <v>297</v>
       </c>
-      <c r="C193" s="194"/>
-      <c r="D193" s="194"/>
-      <c r="E193" s="194"/>
-      <c r="F193" s="195"/>
+      <c r="C193" s="197"/>
+      <c r="D193" s="197"/>
+      <c r="E193" s="197"/>
+      <c r="F193" s="198"/>
       <c r="G193" s="172"/>
       <c r="H193" s="172"/>
       <c r="I193" s="172"/>
@@ -13357,13 +13360,13 @@
     </row>
     <row r="203" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A203" s="31"/>
-      <c r="B203" s="193" t="s">
+      <c r="B203" s="196" t="s">
         <v>307</v>
       </c>
-      <c r="C203" s="194"/>
-      <c r="D203" s="194"/>
-      <c r="E203" s="194"/>
-      <c r="F203" s="195"/>
+      <c r="C203" s="197"/>
+      <c r="D203" s="197"/>
+      <c r="E203" s="197"/>
+      <c r="F203" s="198"/>
       <c r="G203" s="172"/>
       <c r="H203" s="172"/>
       <c r="I203" s="172"/>
@@ -13912,13 +13915,13 @@
     </row>
     <row r="240" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A240" s="31"/>
-      <c r="B240" s="193" t="s">
+      <c r="B240" s="196" t="s">
         <v>340</v>
       </c>
-      <c r="C240" s="194"/>
-      <c r="D240" s="194"/>
-      <c r="E240" s="194"/>
-      <c r="F240" s="195"/>
+      <c r="C240" s="197"/>
+      <c r="D240" s="197"/>
+      <c r="E240" s="197"/>
+      <c r="F240" s="198"/>
       <c r="G240" s="172"/>
       <c r="H240" s="172"/>
       <c r="I240" s="172"/>
@@ -13942,13 +13945,13 @@
     </row>
     <row r="242" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A242" s="31"/>
-      <c r="B242" s="193" t="s">
+      <c r="B242" s="196" t="s">
         <v>342</v>
       </c>
-      <c r="C242" s="194"/>
-      <c r="D242" s="194"/>
-      <c r="E242" s="194"/>
-      <c r="F242" s="195"/>
+      <c r="C242" s="197"/>
+      <c r="D242" s="197"/>
+      <c r="E242" s="197"/>
+      <c r="F242" s="198"/>
       <c r="G242" s="172"/>
       <c r="H242" s="172"/>
       <c r="I242" s="172"/>
@@ -13972,13 +13975,13 @@
     </row>
     <row r="244" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A244" s="31"/>
-      <c r="B244" s="193" t="s">
+      <c r="B244" s="196" t="s">
         <v>344</v>
       </c>
-      <c r="C244" s="194"/>
-      <c r="D244" s="194"/>
-      <c r="E244" s="194"/>
-      <c r="F244" s="195"/>
+      <c r="C244" s="197"/>
+      <c r="D244" s="197"/>
+      <c r="E244" s="197"/>
+      <c r="F244" s="198"/>
       <c r="G244" s="172"/>
       <c r="H244" s="172"/>
       <c r="I244" s="172"/>
@@ -14002,13 +14005,13 @@
     </row>
     <row r="246" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A246" s="31"/>
-      <c r="B246" s="193" t="s">
+      <c r="B246" s="196" t="s">
         <v>346</v>
       </c>
-      <c r="C246" s="194"/>
-      <c r="D246" s="194"/>
-      <c r="E246" s="194"/>
-      <c r="F246" s="195"/>
+      <c r="C246" s="197"/>
+      <c r="D246" s="197"/>
+      <c r="E246" s="197"/>
+      <c r="F246" s="198"/>
       <c r="G246" s="172"/>
       <c r="H246" s="172"/>
       <c r="I246" s="172"/>
@@ -14032,13 +14035,13 @@
     </row>
     <row r="248" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A248" s="31"/>
-      <c r="B248" s="196" t="s">
+      <c r="B248" s="212" t="s">
         <v>348</v>
       </c>
-      <c r="C248" s="194"/>
-      <c r="D248" s="194"/>
-      <c r="E248" s="194"/>
-      <c r="F248" s="195"/>
+      <c r="C248" s="197"/>
+      <c r="D248" s="197"/>
+      <c r="E248" s="197"/>
+      <c r="F248" s="198"/>
       <c r="G248" s="172"/>
       <c r="H248" s="172"/>
       <c r="I248" s="172"/>
@@ -14199,21 +14202,27 @@
       <c r="A259" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="B259" s="192" t="s">
+      <c r="B259" s="211" t="s">
         <v>103</v>
       </c>
-      <c r="C259" s="192"/>
-      <c r="D259" s="192"/>
-      <c r="E259" s="192"/>
-      <c r="F259" s="192"/>
-      <c r="G259" s="192"/>
-      <c r="H259" s="192"/>
-      <c r="I259" s="192"/>
-      <c r="J259" s="192"/>
-      <c r="K259" s="192"/>
+      <c r="C259" s="211"/>
+      <c r="D259" s="211"/>
+      <c r="E259" s="211"/>
+      <c r="F259" s="211"/>
+      <c r="G259" s="211"/>
+      <c r="H259" s="211"/>
+      <c r="I259" s="211"/>
+      <c r="J259" s="211"/>
+      <c r="K259" s="211"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B259:K259"/>
+    <mergeCell ref="B193:F193"/>
+    <mergeCell ref="B248:F248"/>
+    <mergeCell ref="B242:F242"/>
+    <mergeCell ref="B240:F240"/>
+    <mergeCell ref="B203:F203"/>
     <mergeCell ref="G2:K2"/>
     <mergeCell ref="K16:K17"/>
     <mergeCell ref="B246:F246"/>
@@ -14228,12 +14237,6 @@
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="B45:F45"/>
     <mergeCell ref="B153:F153"/>
-    <mergeCell ref="B259:K259"/>
-    <mergeCell ref="B193:F193"/>
-    <mergeCell ref="B248:F248"/>
-    <mergeCell ref="B242:F242"/>
-    <mergeCell ref="B240:F240"/>
-    <mergeCell ref="B203:F203"/>
   </mergeCells>
   <phoneticPr fontId="71"/>
   <pageMargins left="0.77" right="0" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -14257,10 +14260,10 @@
   <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0">
     <tabColor indexed="15"/>
   </sheetPr>
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G208"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="B11" zoomScaleNormal="65" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="65" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="B182" zoomScaleNormal="65" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="65" workbookViewId="0">
+      <selection activeCell="F207" sqref="F207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -14420,6 +14423,11 @@
       <c r="G14" s="119"/>
     </row>
     <row r="24" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="208" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C208" s="127" t="s">
+        <v>354</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A4:B4"/>
@@ -14441,10 +14449,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J335"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A304" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="C330" sqref="C330"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -14516,6 +14524,11 @@
         <v>134</v>
       </c>
       <c r="J4" s="136"/>
+    </row>
+    <row r="335" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C335" s="138" t="s">
+        <v>164</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4"/>

</xml_diff>